<commit_message>
Extent Report Scripts added
</commit_message>
<xml_diff>
--- a/Framework/src/main/resources/com/aspiresys/resources/Github.xlsx
+++ b/Framework/src/main/resources/com/aspiresys/resources/Github.xlsx
@@ -90,9 +90,6 @@
     <t>Y</t>
   </si>
   <si>
-    <t>N</t>
-  </si>
-  <si>
     <t>TC03</t>
   </si>
   <si>
@@ -109,13 +106,16 @@
   </si>
   <si>
     <t>dummy05</t>
+  </si>
+  <si>
+    <t>https://github.com/login04</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -135,6 +135,14 @@
       <color theme="1"/>
       <name val="Courier New"/>
       <family val="3"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -175,10 +183,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -192,8 +201,10 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -496,7 +507,7 @@
   <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -620,7 +631,7 @@
         <v>17</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>4</v>
@@ -650,8 +661,8 @@
         <v>9</v>
       </c>
       <c r="E10" s="3"/>
-      <c r="F10" s="3" t="s">
-        <v>10</v>
+      <c r="F10" s="7" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -696,7 +707,7 @@
     </row>
     <row r="14" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>17</v>
@@ -747,7 +758,7 @@
         <v>11</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -778,13 +789,13 @@
     </row>
     <row r="20" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>17</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>4</v>
@@ -814,8 +825,8 @@
         <v>9</v>
       </c>
       <c r="E22" s="3"/>
-      <c r="F22" s="3" t="s">
-        <v>10</v>
+      <c r="F22" s="7" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -829,7 +840,7 @@
         <v>11</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -860,7 +871,7 @@
     </row>
     <row r="26" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B26" s="4" t="s">
         <v>17</v>
@@ -896,7 +907,7 @@
         <v>9</v>
       </c>
       <c r="E28" s="3"/>
-      <c r="F28" s="3" t="s">
+      <c r="F28" s="7" t="s">
         <v>10</v>
       </c>
     </row>
@@ -911,7 +922,7 @@
         <v>11</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -946,8 +957,13 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F28" r:id="rId1"/>
+    <hyperlink ref="F22" r:id="rId2"/>
+    <hyperlink ref="F10" r:id="rId3"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 

</xml_diff>